<commit_message>
materiaal lisjt update & toevoegen datasheets
</commit_message>
<xml_diff>
--- a/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
+++ b/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Overzichten\Materiaal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Datasheets &amp; Materiaal lijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE1B691-4106-47F8-99A0-DD8544346E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A738C041-2342-42AC-8411-08ECD1B446A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,56 +36,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>drukknoppen</t>
   </si>
   <si>
-    <t>bedrading</t>
-  </si>
-  <si>
-    <t>microcontrollers(arduino)</t>
-  </si>
-  <si>
     <t>behuizing</t>
   </si>
   <si>
     <t>software</t>
   </si>
   <si>
-    <t>Leds</t>
-  </si>
-  <si>
     <t>Fiets</t>
   </si>
   <si>
     <t>Extra info</t>
   </si>
   <si>
-    <t xml:space="preserve">BEC </t>
-  </si>
-  <si>
     <t>Ja</t>
   </si>
   <si>
     <t>Uitbreiding wielspaken verlichting</t>
   </si>
   <si>
-    <t>https://be.farnell.com/multicomp-pro/mc8ms8p1b06vs2qes/switch-spdt-on-mom-v-bracket/dp/2008736</t>
-  </si>
-  <si>
-    <t>Leverancier</t>
-  </si>
-  <si>
-    <t>Farnell</t>
-  </si>
-  <si>
     <t>batterijhouders</t>
   </si>
   <si>
-    <t>breadboard</t>
-  </si>
-  <si>
     <t>Basis</t>
   </si>
   <si>
@@ -107,9 +83,6 @@
     <t>Url</t>
   </si>
   <si>
-    <t>totale kostprijs (incl.btw</t>
-  </si>
-  <si>
     <t>aangevraagd door</t>
   </si>
   <si>
@@ -147,6 +120,66 @@
   </si>
   <si>
     <t>Farnell (automatisch)</t>
+  </si>
+  <si>
+    <t>Arduino® Nano 33 BLE Sense Rev2</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/arduino/abx00035/nano-33-ble-sense-w-header-dev/dp/3404697</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/multicomp/mc32874/tactile-switch-spst-no-0-05a-12v/dp/2543105</t>
+  </si>
+  <si>
+    <t>MC32874</t>
+  </si>
+  <si>
+    <t>Nee</t>
+  </si>
+  <si>
+    <t>BEC (LM2940T-5.0/NOPB)</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/en-BE/texas-instruments/lm2940t-5-0-nopb/ic-v-reg-linear-5v/dp/3122082?MER=BR-MER-CA-RECO-STM71778</t>
+  </si>
+  <si>
+    <t>Led Strips</t>
+  </si>
+  <si>
+    <t>kostprijs (excl.btw)</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/en-BE/bud-industries/bc-32629/jumper-wire-26awg-7-87inch-40pcs/dp/2762507?MER=BR-MER-CA-RECO-STM71778</t>
+  </si>
+  <si>
+    <t>BC-32629  Wires Female</t>
+  </si>
+  <si>
+    <t>BC-32627 wires Male</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/en-BE/bud-industries/bc-32627/jumper-wire-26awg-7-87inch-40pcs/dp/2762506?MER=BR-MER-CA-RECO-STM71778</t>
+  </si>
+  <si>
+    <t>PROTOTYPING BOARD, CEM-3, 100MM X 160MM</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/en-BE/gspk-circuits/gc005-lf/prototyping-board-cem-3-100mm/dp/3263921?MER=BR-MER-CA-RECO-STM71778</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/arduino-abx00070-board-nano-ble-sense-rev2-with-headers-nano-arm-cortex-m4-2740365.html?refresh=true</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>breadboard TW-E40-510 (test boards)</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/en-BE/twin-industries/tw-e40-510/breadboard-solderless-400-tie/dp/2295705?MER=BR-MER-CA-RECO-STM71778</t>
+  </si>
+  <si>
+    <t>JST connector</t>
   </si>
 </sst>
 </file>
@@ -205,21 +238,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -233,29 +341,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}" name="Tabel1" displayName="Tabel1" ref="A2:T22" totalsRowShown="0">
-  <autoFilter ref="A2:T22" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}" name="Tabel1" displayName="Tabel1" ref="A2:T26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A2:T26" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{1B5DBAEF-1276-450F-A9EA-3F4E61E1B2D4}" name="Aantal nodig"/>
-    <tableColumn id="20" xr3:uid="{B5B5338E-5671-42DF-BCC5-235E2DA36C6E}" name="Datasheets OK"/>
-    <tableColumn id="19" xr3:uid="{3A981EB3-0FB2-45F3-A4F5-7F05C2ABE0D3}" name="Extra info"/>
-    <tableColumn id="18" xr3:uid="{76C77F8A-EF04-4113-8E13-24A5F4207CBE}" name="Op school"/>
-    <tableColumn id="17" xr3:uid="{D3820DBB-33B7-467C-8237-68B379639303}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{629D7B1D-8050-4C75-B620-C226B56065E5}" name="Datum aanvraag"/>
-    <tableColumn id="8" xr3:uid="{8B66298D-DF14-4969-A852-7F6A53B8671A}" name="aantal te kopen"/>
-    <tableColumn id="3" xr3:uid="{A4DC773C-F033-4DA0-AA0D-B21739089B2C}" name="Korte omschrijving"/>
-    <tableColumn id="4" xr3:uid="{80982AC6-7BD3-4773-8CEC-D400BD08E6CB}" name="winkel"/>
-    <tableColumn id="5" xr3:uid="{DF4EED70-3D1C-446A-91B1-86731E303698}" name="artikelnummer"/>
-    <tableColumn id="6" xr3:uid="{8EF30C82-0B38-42F2-A1A5-6BB9095E8F15}" name="Url"/>
-    <tableColumn id="7" xr3:uid="{FF7045BD-D9BB-444D-8D56-68AA70D9628C}" name="totale kostprijs (incl.btw"/>
-    <tableColumn id="9" xr3:uid="{53EB471E-22EB-4906-9B64-30A34F3E6795}" name="aangevraagd door"/>
-    <tableColumn id="10" xr3:uid="{B838CE0E-9878-4953-9861-A4E298EF8B4A}" name="aantal dagen levertijd"/>
-    <tableColumn id="11" xr3:uid="{BC7D534F-CEFE-41B5-88EE-DF3BAD892082}" name="goedgekeurd door coach"/>
-    <tableColumn id="12" xr3:uid="{EFB61E7F-CB49-4F99-BC3D-EAF55D151363}" name="bestelling ingegeven (RQ-nummer)"/>
-    <tableColumn id="13" xr3:uid="{628EB96F-9E86-4D86-B287-5C4CF675AA17}" name="bestelling door financ dienst geplaats"/>
-    <tableColumn id="14" xr3:uid="{CE0EFD78-769C-4E49-9513-E6214469CD12}" name="bestelling verzonden(verwachte aankomst"/>
-    <tableColumn id="15" xr3:uid="{5DE6143D-3D33-4B5A-AFC0-B70BB8C2156F}" name="bestelling ontvangen(datum)"/>
-    <tableColumn id="16" xr3:uid="{26B2E2E1-82AB-46B3-A25C-EEEBCE8B8487}" name="opmerkingen"/>
+    <tableColumn id="1" xr3:uid="{1B5DBAEF-1276-450F-A9EA-3F4E61E1B2D4}" name="Aantal nodig" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{B5B5338E-5671-42DF-BCC5-235E2DA36C6E}" name="Datasheets OK" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{3A981EB3-0FB2-45F3-A4F5-7F05C2ABE0D3}" name="Extra info" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{76C77F8A-EF04-4113-8E13-24A5F4207CBE}" name="Op school" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{D3820DBB-33B7-467C-8237-68B379639303}" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{629D7B1D-8050-4C75-B620-C226B56065E5}" name="Datum aanvraag" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{8B66298D-DF14-4969-A852-7F6A53B8671A}" name="aantal te kopen" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{A4DC773C-F033-4DA0-AA0D-B21739089B2C}" name="Korte omschrijving" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{80982AC6-7BD3-4773-8CEC-D400BD08E6CB}" name="winkel" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DF4EED70-3D1C-446A-91B1-86731E303698}" name="artikelnummer" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{8EF30C82-0B38-42F2-A1A5-6BB9095E8F15}" name="Url" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{FF7045BD-D9BB-444D-8D56-68AA70D9628C}" name="kostprijs (excl.btw)" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{53EB471E-22EB-4906-9B64-30A34F3E6795}" name="aangevraagd door" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{B838CE0E-9878-4953-9861-A4E298EF8B4A}" name="aantal dagen levertijd" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{BC7D534F-CEFE-41B5-88EE-DF3BAD892082}" name="goedgekeurd door coach" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{EFB61E7F-CB49-4F99-BC3D-EAF55D151363}" name="bestelling ingegeven (RQ-nummer)" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{628EB96F-9E86-4D86-B287-5C4CF675AA17}" name="bestelling door financ dienst geplaats" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{CE0EFD78-769C-4E49-9513-E6214469CD12}" name="bestelling verzonden(verwachte aankomst" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{5DE6143D-3D33-4B5A-AFC0-B70BB8C2156F}" name="bestelling ontvangen(datum)" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{26B2E2E1-82AB-46B3-A25C-EEEBCE8B8487}" name="opmerkingen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -524,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:T18"/>
+  <dimension ref="A2:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,192 +646,789 @@
     <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" customWidth="1"/>
+    <col min="11" max="11" width="15.90625" customWidth="1"/>
     <col min="12" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="R2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="S2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="T2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
       <c r="E5" s="2"/>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="G6">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>9</v>
-      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H7" t="s">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H8" t="s">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H9" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H10" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.97</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="5">
+        <v>7800</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="5">
+        <v>6880</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="5">
+        <v>7770</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="5">
+        <v>5380</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G18">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
         <v>0</v>
       </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" s="3">
+        <v>46.99</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" xr:uid="{24ADC868-2AAA-4DCB-A9D8-FF154C0B2CC5}"/>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{30B1C237-5E69-4C1D-9F34-690763FA92C2}"/>
+    <hyperlink ref="K6" r:id="rId2" xr:uid="{813D217E-89BC-47F3-90F0-137686EADA35}"/>
+    <hyperlink ref="K11" r:id="rId3" xr:uid="{844A1DDE-804C-468E-A328-66583EFA6EEA}"/>
+    <hyperlink ref="K13" r:id="rId4" xr:uid="{1B3102BE-8A53-40A7-8E74-F152EEE70D5C}"/>
+    <hyperlink ref="K14" r:id="rId5" xr:uid="{65DB326A-5E31-4AC1-B0E8-FFDC774BF9EC}"/>
+    <hyperlink ref="K15" r:id="rId6" xr:uid="{8A8201DB-F08F-47EB-92D9-73166B0936D6}"/>
+    <hyperlink ref="K20" r:id="rId7" xr:uid="{A5BA04AF-FA81-447D-90B0-B9C36D6494C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
materiaal lijst update + nieuwe datasheets + invullen aankoop lijst
</commit_message>
<xml_diff>
--- a/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
+++ b/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Datasheets &amp; Materiaal lijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A738C041-2342-42AC-8411-08ECD1B446A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E110B3-E764-4360-92B4-5C90D3784729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>drukknoppen</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Uitbreiding wielspaken verlichting</t>
   </si>
   <si>
-    <t>batterijhouders</t>
-  </si>
-  <si>
     <t>Basis</t>
   </si>
   <si>
@@ -179,7 +176,34 @@
     <t>https://be.farnell.com/en-BE/twin-industries/tw-e40-510/breadboard-solderless-400-tie/dp/2295705?MER=BR-MER-CA-RECO-STM71778</t>
   </si>
   <si>
-    <t>JST connector</t>
+    <t>Niet nodig</t>
+  </si>
+  <si>
+    <t>JST connector of algemene connectors</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/nidec-copal/mfs201n-z/slide-switch-dpdt-1a-125vac-panel/dp/2854848?MER=BR-MER-CA-RECO-STM71778</t>
+  </si>
+  <si>
+    <t>Batterijen zelf (LI-ION) 8</t>
+  </si>
+  <si>
+    <t>Batterij houders</t>
+  </si>
+  <si>
+    <t>https://opencircuit.nl/product/battery-holder-2x18650-wire-leads</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>opencircuit</t>
+  </si>
+  <si>
+    <t>Aan uit switch  voeding</t>
+  </si>
+  <si>
+    <t>2740365 - 62</t>
   </si>
 </sst>
 </file>
@@ -341,8 +365,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}" name="Tabel1" displayName="Tabel1" ref="A2:T26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A2:T26" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}" name="Tabel1" displayName="Tabel1" ref="A2:T29" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A2:T29" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{1B5DBAEF-1276-450F-A9EA-3F4E61E1B2D4}" name="Aantal nodig" dataDxfId="19"/>
     <tableColumn id="20" xr3:uid="{B5B5338E-5671-42DF-BCC5-235E2DA36C6E}" name="Datasheets OK" dataDxfId="18"/>
@@ -632,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:T26"/>
+  <dimension ref="A2:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,69 +680,69 @@
   <sheetData>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -757,14 +781,14 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -776,29 +800,35 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.3</v>
+      </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -810,32 +840,30 @@
     </row>
     <row r="6" spans="1:20" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="3">
-        <v>0.3</v>
+        <v>15.99</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -846,29 +874,33 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="3">
+        <v>60156</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2.65</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -878,28 +910,30 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -915,11 +949,11 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -927,11 +961,11 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -947,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -959,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -974,33 +1008,29 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="3">
-        <v>1.97</v>
-      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -1010,33 +1040,29 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" s="5">
-        <v>7800</v>
-      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -1046,32 +1072,34 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="116" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="5">
-        <v>6880</v>
+        <v>33</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.97</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -1082,9 +1110,9 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="116" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
@@ -1094,20 +1122,20 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" s="3"/>
-      <c r="K14" s="4" t="s">
-        <v>40</v>
+      <c r="K14" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="L14" s="5">
-        <v>7770</v>
+        <v>7800</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1118,30 +1146,32 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="145" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L15" s="5">
-        <v>5380</v>
+        <v>6880</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -1152,21 +1182,33 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+    <row r="16" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
       <c r="H16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="5">
+        <v>7770</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -1176,19 +1218,33 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+    <row r="17" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="5">
+        <v>5380</v>
+      </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1209,8 +1265,8 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -1228,13 +1284,13 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="2" t="s">
-        <v>6</v>
+      <c r="H19" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1244,35 +1300,19 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="3">
-        <v>46.99</v>
-      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1283,11 +1323,11 @@
       <c r="T20" s="3"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1304,7 +1344,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1312,7 +1352,9 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1326,19 +1368,35 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+    <row r="23" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="K23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="3">
+        <v>46.99</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -1349,11 +1407,11 @@
       <c r="T23" s="3"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1414,21 +1472,90 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" xr:uid="{30B1C237-5E69-4C1D-9F34-690763FA92C2}"/>
-    <hyperlink ref="K6" r:id="rId2" xr:uid="{813D217E-89BC-47F3-90F0-137686EADA35}"/>
-    <hyperlink ref="K11" r:id="rId3" xr:uid="{844A1DDE-804C-468E-A328-66583EFA6EEA}"/>
-    <hyperlink ref="K13" r:id="rId4" xr:uid="{1B3102BE-8A53-40A7-8E74-F152EEE70D5C}"/>
-    <hyperlink ref="K14" r:id="rId5" xr:uid="{65DB326A-5E31-4AC1-B0E8-FFDC774BF9EC}"/>
-    <hyperlink ref="K15" r:id="rId6" xr:uid="{8A8201DB-F08F-47EB-92D9-73166B0936D6}"/>
-    <hyperlink ref="K20" r:id="rId7" xr:uid="{A5BA04AF-FA81-447D-90B0-B9C36D6494C4}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{813D217E-89BC-47F3-90F0-137686EADA35}"/>
+    <hyperlink ref="K13" r:id="rId3" xr:uid="{844A1DDE-804C-468E-A328-66583EFA6EEA}"/>
+    <hyperlink ref="K15" r:id="rId4" xr:uid="{1B3102BE-8A53-40A7-8E74-F152EEE70D5C}"/>
+    <hyperlink ref="K16" r:id="rId5" xr:uid="{65DB326A-5E31-4AC1-B0E8-FFDC774BF9EC}"/>
+    <hyperlink ref="K17" r:id="rId6" xr:uid="{8A8201DB-F08F-47EB-92D9-73166B0936D6}"/>
+    <hyperlink ref="K23" r:id="rId7" xr:uid="{A5BA04AF-FA81-447D-90B0-B9C36D6494C4}"/>
+    <hyperlink ref="K8" r:id="rId8" xr:uid="{A5040F13-6C7E-4751-9A3B-4BFBF382143F}"/>
+    <hyperlink ref="K6" r:id="rId9" xr:uid="{CF341961-DC55-42A8-8A49-C5AC4E242DFB}"/>
+    <hyperlink ref="K7" r:id="rId10" xr:uid="{E4F33FE5-5923-40B7-BC8B-C0C00E95631A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bestellijst aangevuld & pdf's van componenten aangevuld
</commit_message>
<xml_diff>
--- a/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
+++ b/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Datasheets &amp; Materiaal lijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E110B3-E764-4360-92B4-5C90D3784729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA76AC1E-2E62-4D81-B13D-38AC55CCF662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>drukknoppen</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Niet nodig</t>
   </si>
   <si>
-    <t>JST connector of algemene connectors</t>
-  </si>
-  <si>
     <t>https://be.farnell.com/nidec-copal/mfs201n-z/slide-switch-dpdt-1a-125vac-panel/dp/2854848?MER=BR-MER-CA-RECO-STM71778</t>
   </si>
   <si>
@@ -204,6 +201,24 @@
   </si>
   <si>
     <t>2740365 - 62</t>
+  </si>
+  <si>
+    <t>TP4056 USB-C Li-ion lader 1A met Li-ion protection circuit</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/nl/power/bms-en-laders/li-ion-en-li-po/met-protectiecircuit/tp4056-usb-c-li-ion-lader-1a-met-li-ion-protection-circuit</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>tinytronics</t>
+  </si>
+  <si>
+    <t>ST-SM 3p connector kabel- 30cm</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/nl/verlichting/led-strips/accessoires/jst-sm-3p-compatible-verlengkabel-30cm</t>
   </si>
 </sst>
 </file>
@@ -658,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -853,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>43</v>
@@ -887,16 +902,16 @@
         <v>3</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="3">
         <v>60156</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="3">
         <v>2.65</v>
@@ -923,16 +938,16 @@
         <v>4</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1194,7 +1209,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>38</v>
@@ -1254,19 +1269,33 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5"/>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2151</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -1276,21 +1305,33 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+    <row r="19" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3">
+        <v>6</v>
+      </c>
       <c r="H19" s="3" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
+      <c r="J19" s="3">
+        <v>3580</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="5">
+        <v>12</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1551,11 +1592,13 @@
     <hyperlink ref="K8" r:id="rId8" xr:uid="{A5040F13-6C7E-4751-9A3B-4BFBF382143F}"/>
     <hyperlink ref="K6" r:id="rId9" xr:uid="{CF341961-DC55-42A8-8A49-C5AC4E242DFB}"/>
     <hyperlink ref="K7" r:id="rId10" xr:uid="{E4F33FE5-5923-40B7-BC8B-C0C00E95631A}"/>
+    <hyperlink ref="K18" r:id="rId11" xr:uid="{ED3872C5-9143-40BC-9373-9E0F69590981}"/>
+    <hyperlink ref="K19" r:id="rId12" xr:uid="{D75B5948-5920-4534-8C2E-E90A74B3C724}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update magteriaal lijst geleverde goederen - connector  kabels
</commit_message>
<xml_diff>
--- a/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
+++ b/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Datasheets &amp; Materiaal lijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA76AC1E-2E62-4D81-B13D-38AC55CCF662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76343FFA-754A-4931-9798-5DA4CE17F4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>drukknoppen</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>https://www.tinytronics.nl/nl/verlichting/led-strips/accessoires/jst-sm-3p-compatible-verlengkabel-30cm</t>
+  </si>
+  <si>
+    <t>Afgekeurd voor aankoop</t>
+  </si>
+  <si>
+    <t>N.v.t</t>
   </si>
 </sst>
 </file>
@@ -277,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -294,6 +300,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,7 +390,16 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}" name="Tabel1" displayName="Tabel1" ref="A2:T29" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A2:T29" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}"/>
+  <autoFilter ref="A2:T29" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}">
+    <filterColumn colId="6">
+      <filters blank="1">
+        <filter val="1"/>
+        <filter val="3"/>
+        <filter val="4"/>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{1B5DBAEF-1276-450F-A9EA-3F4E61E1B2D4}" name="Aantal nodig" dataDxfId="19"/>
     <tableColumn id="20" xr3:uid="{B5B5338E-5671-42DF-BCC5-235E2DA36C6E}" name="Datasheets OK" dataDxfId="18"/>
@@ -673,27 +691,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="15.90625" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -755,7 +774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -779,7 +798,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -815,7 +834,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -825,7 +844,9 @@
         <v>0</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="6">
+        <v>46065</v>
+      </c>
       <c r="G5" s="3">
         <v>6</v>
       </c>
@@ -853,7 +874,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -889,7 +910,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -897,7 +918,9 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="6">
+        <v>46065</v>
+      </c>
       <c r="G7" s="3">
         <v>3</v>
       </c>
@@ -925,7 +948,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -933,7 +956,9 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="6">
+        <v>46065</v>
+      </c>
       <c r="G8" s="3">
         <v>4</v>
       </c>
@@ -959,7 +984,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -991,7 +1016,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1023,7 +1048,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -1055,7 +1080,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1087,7 +1112,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -1125,7 +1150,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -1161,7 +1186,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -1197,17 +1222,21 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="144" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="6">
+        <v>46065</v>
+      </c>
       <c r="G16" s="3">
         <v>1</v>
       </c>
@@ -1230,10 +1259,12 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
+      <c r="S16" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -1269,7 +1300,7 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" ht="145" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -1277,7 +1308,9 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="6">
+        <v>46065</v>
+      </c>
       <c r="G18" s="3">
         <v>3</v>
       </c>
@@ -1305,7 +1338,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" ht="116" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -1315,7 +1348,9 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="6">
+        <v>46065</v>
+      </c>
       <c r="G19" s="3">
         <v>6</v>
       </c>
@@ -1338,10 +1373,12 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="6">
+        <v>46079</v>
+      </c>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1363,7 +1400,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1385,7 +1422,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1409,7 +1446,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>1</v>
       </c>
@@ -1421,7 +1458,9 @@
         <v>0</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="6">
+        <v>46065</v>
+      </c>
       <c r="G23" s="3">
         <v>1</v>
       </c>
@@ -1447,7 +1486,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1469,7 +1508,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1491,7 +1530,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1513,7 +1552,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1535,7 +1574,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1557,7 +1596,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>

</xml_diff>

<commit_message>
Datasheets & Materiaal lijst mappen namen update's & onvangen componenten binnen nemen in materiaal lijst
</commit_message>
<xml_diff>
--- a/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
+++ b/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Datasheets &amp; Materiaal lijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76343FFA-754A-4931-9798-5DA4CE17F4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90900872-E838-4526-83C3-99D7FF46F5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>drukknoppen</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>N.v.t</t>
+  </si>
+  <si>
+    <t>Uit bestelijst exele gehaald 12/02/2026</t>
   </si>
 </sst>
 </file>
@@ -390,16 +393,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}" name="Tabel1" displayName="Tabel1" ref="A2:T29" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A2:T29" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}">
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="1"/>
-        <filter val="3"/>
-        <filter val="4"/>
-        <filter val="6"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:T29" xr:uid="{FF0E2E08-0CB4-41D1-909A-9866F9E2FAC5}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{1B5DBAEF-1276-450F-A9EA-3F4E61E1B2D4}" name="Aantal nodig" dataDxfId="19"/>
     <tableColumn id="20" xr3:uid="{B5B5338E-5671-42DF-BCC5-235E2DA36C6E}" name="Datasheets OK" dataDxfId="18"/>
@@ -691,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,7 +792,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -871,10 +865,12 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="S5" s="6">
+        <v>46079</v>
+      </c>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -981,10 +977,12 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="S8" s="6">
+        <v>46079</v>
+      </c>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -1016,7 +1014,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1048,7 +1046,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -1080,7 +1078,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1112,7 +1110,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -1150,7 +1148,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -1186,7 +1184,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="144" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -1264,7 +1262,7 @@
       </c>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -1304,7 +1302,9 @@
       <c r="A18" s="3">
         <v>3</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1335,7 +1335,9 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="S18" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="T18" s="3"/>
     </row>
     <row r="19" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
10-pins vrouwelijke 11 mm hoge stapelbare headerconnector (OT3782) in materiaal lijst gezet
</commit_message>
<xml_diff>
--- a/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
+++ b/Documentatie/Datasheets & Materiaal lijst/Materiaal lijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\PX1 - BrakeNBlink\BrakeNBlink\Documentatie\Datasheets &amp; Materiaal lijst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90900872-E838-4526-83C3-99D7FF46F5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB588E8-081F-4F71-BD64-E4294E8D7319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>drukknoppen</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>Uit bestelijst exele gehaald 12/02/2026</t>
+  </si>
+  <si>
+    <t>10-pins vrouwelijke 11 mm hoge stapelbare headerconnector (OT3782)</t>
+  </si>
+  <si>
+    <t>https://www.otronic.nl/nl/10-pins-vrouwelijke-11-mm-hoge-stapelbare-headerco.html</t>
   </si>
 </sst>
 </file>
@@ -685,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,19 +1386,29 @@
       </c>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="6">
+        <v>46065</v>
+      </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
+      <c r="K20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" s="5">
+        <v>12</v>
+      </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1635,11 +1651,12 @@
     <hyperlink ref="K7" r:id="rId10" xr:uid="{E4F33FE5-5923-40B7-BC8B-C0C00E95631A}"/>
     <hyperlink ref="K18" r:id="rId11" xr:uid="{ED3872C5-9143-40BC-9373-9E0F69590981}"/>
     <hyperlink ref="K19" r:id="rId12" xr:uid="{D75B5948-5920-4534-8C2E-E90A74B3C724}"/>
+    <hyperlink ref="K20" r:id="rId13" xr:uid="{61D311D3-CA8B-4426-92A1-9418C7E9F48B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>